<commit_message>
Add New Event & Get Event api implemented
</commit_message>
<xml_diff>
--- a/GurukulAppAdminPanel/docs/API_DOCUMENT.xlsx
+++ b/GurukulAppAdminPanel/docs/API_DOCUMENT.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="58">
   <si>
     <t>Sl. No</t>
   </si>
@@ -30,18 +30,6 @@
     <t>http:///</t>
   </si>
   <si>
-    <t>api/get-module-data</t>
-  </si>
-  <si>
-    <t>http://dragapi.tangenttechsolutions.com/</t>
-  </si>
-  <si>
-    <t>Get ModuleData</t>
-  </si>
-  <si>
-    <t>USP_END_USER_ACTIVITY</t>
-  </si>
-  <si>
     <t>Procedure Name</t>
   </si>
   <si>
@@ -70,13 +58,145 @@
   </si>
   <si>
     <t>Prod</t>
+  </si>
+  <si>
+    <t>JSON</t>
+  </si>
+  <si>
+    <t>http://gurukulweb.tangenttechsolutions.com</t>
+  </si>
+  <si>
+    <t>api/volunteer-event-checkinout-update</t>
+  </si>
+  <si>
+    <t>api/itinary-status-update</t>
+  </si>
+  <si>
+    <t>POST</t>
+  </si>
+  <si>
+    <t>Update Check In Out Date</t>
+  </si>
+  <si>
+    <t>USP_EVENT_MANAGEMENT</t>
+  </si>
+  <si>
+    <t>update check-in-out_date</t>
+  </si>
+  <si>
+    <t>[{"STATUS":"26","CHECKIN_DATE":"01-12-2018 ","CHECKIN_TIME":"11:39 AM","CHECKOUT_DATE":"16-12-2018","CHECKOUT_TIME":"6:40 PM","EVENT_ID":"1","USER_ID":"50","MESSAGE":80}]</t>
+  </si>
+  <si>
+    <t>[{"ID_CARD_TYPE":"","TRANSPORTAION_ARRANGEMENT":"","ACCOMODATION_ARRANGEMENT":"","EVENT_REG_ID":""}]</t>
+  </si>
+  <si>
+    <t>itinerary-satatus-update</t>
+  </si>
+  <si>
+    <t>api/topic-status-update</t>
+  </si>
+  <si>
+    <t>Topic Status Update</t>
+  </si>
+  <si>
+    <t>[{"TOPIC_STATUS":"","COMMENT_FOR_HOD":"""EVENT_REG_SYS_ID":""}]</t>
+  </si>
+  <si>
+    <t>api/user-login</t>
+  </si>
+  <si>
+    <t>User Login</t>
+  </si>
+  <si>
+    <t>USP_AUTHENTICATE_MANAGEMENT</t>
+  </si>
+  <si>
+    <t>login</t>
+  </si>
+  <si>
+    <t>api/event-registration-cancel</t>
+  </si>
+  <si>
+    <t>Event reg cancel</t>
+  </si>
+  <si>
+    <t>[{"USER_ID":"44","EVENT_ID":"32"}]</t>
+  </si>
+  <si>
+    <t>Event Registration Cancel</t>
+  </si>
+  <si>
+    <t>api/event-registration</t>
+  </si>
+  <si>
+    <t>Event Registration</t>
+  </si>
+  <si>
+    <t>[{"EVENT_SYS_ID":"4","USER_ID":"50","EVENT_TYPE":"2","START_DATE":"11/01/2018","END_DATE":"12/01/2018","COMMENT":"","CLASSID":""}]</t>
+  </si>
+  <si>
+    <t>api/update-user-status</t>
+  </si>
+  <si>
+    <t>Update User Status</t>
+  </si>
+  <si>
+    <t>USP_USERS_MANAGEMENT</t>
+  </si>
+  <si>
+    <t>delete-coaching-detail</t>
+  </si>
+  <si>
+    <t>DELETE</t>
+  </si>
+  <si>
+    <t>Delete Ias Coaching</t>
+  </si>
+  <si>
+    <t>api/update-user-profile</t>
+  </si>
+  <si>
+    <t>Update User Profile</t>
+  </si>
+  <si>
+    <t>api/get-registered-event-data?event_id=</t>
+  </si>
+  <si>
+    <t>Get Registered Event Data</t>
+  </si>
+  <si>
+    <t>view registered event data</t>
+  </si>
+  <si>
+    <t>api/get-user-data?user_id=</t>
+  </si>
+  <si>
+    <t>Get User List</t>
+  </si>
+  <si>
+    <t>api/get-coaching-detail-data</t>
+  </si>
+  <si>
+    <t>Get Coaching Detail Data</t>
+  </si>
+  <si>
+    <t>api/update-coaching-detail</t>
+  </si>
+  <si>
+    <t>Update Coaching Detail</t>
+  </si>
+  <si>
+    <t>api/add-coaching-detail</t>
+  </si>
+  <si>
+    <t>Add Coaching Detail</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -100,14 +220,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -122,6 +234,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF505050"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF505050"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -131,7 +256,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -183,6 +308,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -191,22 +327,21 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -219,6 +354,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -514,10 +656,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -537,53 +679,53 @@
     </row>
     <row r="2" spans="1:8" ht="16.5" customHeight="1">
       <c r="B2" s="5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="8"/>
+        <v>10</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="7"/>
       <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:8" ht="16.5" customHeight="1">
-      <c r="B3" s="9"/>
+      <c r="B3" s="8"/>
       <c r="C3" s="5" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="10"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="9"/>
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="11"/>
-      <c r="B4" s="12"/>
+      <c r="A4" s="10"/>
+      <c r="B4" s="11"/>
       <c r="C4" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
+        <v>12</v>
+      </c>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="11"/>
-      <c r="B5" s="12"/>
+      <c r="A5" s="10"/>
+      <c r="B5" s="11"/>
       <c r="C5" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
+        <v>13</v>
+      </c>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
     </row>
@@ -592,171 +734,352 @@
         <v>0</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="H6" s="13"/>
+      <c r="H6" s="12" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="7" spans="1:8" ht="15.75">
-      <c r="A7" s="7">
+      <c r="A7" s="6">
         <v>1</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="15">
         <v>6</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="G7" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7" s="18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15.75">
+      <c r="A8" s="6">
+        <v>2</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="13">
+        <v>28</v>
+      </c>
+      <c r="G8" s="6"/>
+      <c r="H8" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15.75">
+      <c r="A9" s="6">
+        <v>3</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="13">
+        <v>27</v>
+      </c>
+      <c r="G9" s="6"/>
+      <c r="H9" s="12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15.75">
+      <c r="A10" s="6">
+        <v>4</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" s="13">
+        <v>1</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H10" s="12"/>
+    </row>
+    <row r="11" spans="1:8" ht="15.75">
+      <c r="A11" s="6">
+        <v>5</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" s="13">
+        <v>12</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="H11" s="12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15.75">
+      <c r="A12" s="6">
+        <v>6</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" s="13">
+        <v>2</v>
+      </c>
+      <c r="G12" s="6"/>
+      <c r="H12" s="12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15.75">
+      <c r="A13" s="6">
+        <v>7</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F13" s="13">
+        <v>6</v>
+      </c>
+      <c r="G13" s="6"/>
+      <c r="H13" s="12"/>
+    </row>
+    <row r="14" spans="1:8" ht="15.75">
+      <c r="A14" s="6">
+        <v>8</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F14" s="13">
+        <v>26</v>
+      </c>
+      <c r="G14" s="6"/>
+      <c r="H14" s="12"/>
+    </row>
+    <row r="15" spans="1:8" ht="15.75">
+      <c r="A15" s="6">
         <v>9</v>
       </c>
-      <c r="D7" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="E7" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="F7" s="16">
-        <v>1</v>
-      </c>
-      <c r="G7" s="7"/>
-      <c r="H7" s="3"/>
-    </row>
-    <row r="8" spans="1:8" ht="15.75">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="13"/>
-    </row>
-    <row r="9" spans="1:8" ht="15.75">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="13"/>
-    </row>
-    <row r="10" spans="1:8" ht="15.75">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="13"/>
-    </row>
-    <row r="11" spans="1:8" ht="15.75">
-      <c r="A11" s="7"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="13"/>
-    </row>
-    <row r="12" spans="1:8" ht="15.75">
-      <c r="A12" s="7"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="13"/>
-    </row>
-    <row r="13" spans="1:8" ht="15.75">
-      <c r="A13" s="7"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="13"/>
-    </row>
-    <row r="14" spans="1:8" ht="15.75">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="13"/>
-    </row>
-    <row r="15" spans="1:8" ht="15.75">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="14"/>
+      <c r="B15" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F15" s="13">
+        <v>5</v>
+      </c>
       <c r="G15" s="4"/>
       <c r="H15" s="1"/>
     </row>
     <row r="16" spans="1:8" ht="15.75">
-      <c r="A16" s="7"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="4"/>
+      <c r="A16" s="6">
+        <v>10</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F16" s="13">
+        <v>25</v>
+      </c>
+      <c r="G16" s="21" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="17" spans="1:7" ht="15.75">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="14"/>
+      <c r="A17" s="6">
+        <v>11</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F17" s="13">
+        <v>4</v>
+      </c>
       <c r="G17" s="4"/>
     </row>
     <row r="18" spans="1:7" ht="15.75">
-      <c r="A18" s="7"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="14"/>
+      <c r="A18" s="6">
+        <v>12</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F18" s="13">
+        <v>23</v>
+      </c>
       <c r="G18" s="4"/>
     </row>
     <row r="19" spans="1:7" ht="15.75">
-      <c r="A19" s="7"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="14"/>
+      <c r="A19" s="6">
+        <v>13</v>
+      </c>
+      <c r="B19" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E19" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F19" s="13">
+        <v>22</v>
+      </c>
       <c r="G19" s="4"/>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="14"/>
+      <c r="A20" s="4">
+        <v>14</v>
+      </c>
+      <c r="B20" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E20" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F20" s="13">
+        <v>21</v>
+      </c>
       <c r="G20" s="4"/>
+    </row>
+    <row r="21" spans="1:7" ht="15.75">
+      <c r="A21" s="22">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
master data changes done, booking info share & confirm work done, dashboard count show done
</commit_message>
<xml_diff>
--- a/GurukulAppAdminPanel/docs/API_DOCUMENT.xlsx
+++ b/GurukulAppAdminPanel/docs/API_DOCUMENT.xlsx
@@ -231,9 +231,6 @@
     <t>delete-coaching-detail?Record_ld=</t>
   </si>
   <si>
-    <t>api/get-approved-event-data</t>
-  </si>
-  <si>
     <t>View Approved Event Data</t>
   </si>
   <si>
@@ -313,6 +310,9 @@
   </si>
   <si>
     <t>api/get-content-data?event_reg_id=11</t>
+  </si>
+  <si>
+    <t>api/get-approved-event-data?user_id=</t>
   </si>
 </sst>
 </file>
@@ -795,7 +795,7 @@
   <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -928,17 +928,17 @@
         <v>17</v>
       </c>
       <c r="D8" s="23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E8" s="14" t="s">
         <v>19</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G8" s="6"/>
       <c r="H8" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15.75">
@@ -964,7 +964,7 @@
         <v>28</v>
       </c>
       <c r="H9" s="12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.75">
@@ -1037,10 +1037,10 @@
         <v>6</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H12" s="12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="15.75">
@@ -1063,7 +1063,7 @@
         <v>26</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H13" s="12"/>
     </row>
@@ -1200,7 +1200,7 @@
       </c>
       <c r="G19" s="4"/>
       <c r="H19" s="25" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="15.75">
@@ -1208,7 +1208,7 @@
         <v>14</v>
       </c>
       <c r="B20" s="21" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C20" s="21" t="s">
         <v>5</v>
@@ -1260,7 +1260,7 @@
         <v>5</v>
       </c>
       <c r="D22" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>60</v>
@@ -1272,7 +1272,7 @@
         <v>61</v>
       </c>
       <c r="H22" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="15.75">
@@ -1321,7 +1321,7 @@
         <v>66</v>
       </c>
       <c r="H24" s="24" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="15.75">
@@ -1329,13 +1329,13 @@
         <v>19</v>
       </c>
       <c r="B25" s="21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C25" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="D25" s="2" t="s">
-        <v>71</v>
+      <c r="D25" t="s">
+        <v>98</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>19</v>
@@ -1344,7 +1344,7 @@
         <v>7</v>
       </c>
       <c r="G25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="15.75">
@@ -1352,13 +1352,13 @@
         <v>20</v>
       </c>
       <c r="B26" s="21" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C26" s="21" t="s">
         <v>5</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>19</v>
@@ -1367,7 +1367,7 @@
         <v>8</v>
       </c>
       <c r="G26" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="15.75">
@@ -1375,13 +1375,13 @@
         <v>21</v>
       </c>
       <c r="B27" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C27" s="21" t="s">
         <v>5</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>19</v>
@@ -1390,7 +1390,7 @@
         <v>9</v>
       </c>
       <c r="G27" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="15.75">
@@ -1398,13 +1398,13 @@
         <v>22</v>
       </c>
       <c r="B28" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C28" s="21" t="s">
         <v>17</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>19</v>
@@ -1413,7 +1413,7 @@
         <v>28</v>
       </c>
       <c r="G28" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H28" s="24" t="s">
         <v>22</v>
@@ -1424,7 +1424,7 @@
         <v>23</v>
       </c>
       <c r="B29" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C29" s="21" t="s">
         <v>17</v>
@@ -1439,10 +1439,10 @@
         <v>27</v>
       </c>
       <c r="G29" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H29" s="24" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="15.75">
@@ -1450,13 +1450,13 @@
         <v>24</v>
       </c>
       <c r="B30" s="21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C30" s="21" t="s">
         <v>5</v>
       </c>
       <c r="D30" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>19</v>
@@ -1470,13 +1470,13 @@
         <v>25</v>
       </c>
       <c r="B31" s="21" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C31" s="21" t="s">
         <v>5</v>
       </c>
       <c r="D31" s="19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
All modifications of gurukul
</commit_message>
<xml_diff>
--- a/GurukulAppAdminPanel/docs/API_DOCUMENT.xlsx
+++ b/GurukulAppAdminPanel/docs/API_DOCUMENT.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="103">
   <si>
     <t>Sl. No</t>
   </si>
@@ -316,6 +316,15 @@
   </si>
   <si>
     <t>[{"TOPIC_STATUS":"98","COMMENT_FOR_HOD":"NICE","EVENT_REG_SYS_ID":"12","STATUS":30,"TOPIC_ID":"85"}]</t>
+  </si>
+  <si>
+    <t>User Registration</t>
+  </si>
+  <si>
+    <t>api/user-registration</t>
+  </si>
+  <si>
+    <t>{"TITLE":"12","NAME":"Sujata Kumari","GENDER":"FEMALE","DOB":"27-12-1997","EMAIL":"sujata@tts.com","CONTACT":"9988665533","PASSWORD":"pass","COUNTRY":"104","CITY":"67","COUNTRY_CODE":"+91","CHAPTER":"New Chapter Test","EDUCATION":"","ACTIVITY":"hi"}</t>
   </si>
 </sst>
 </file>
@@ -795,10 +804,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1489,6 +1498,32 @@
       </c>
       <c r="G31" s="2" t="s">
         <v>98</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="15.75">
+      <c r="A32" s="21">
+        <v>26</v>
+      </c>
+      <c r="B32" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C32" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="D32" t="s">
+        <v>101</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F32" s="22">
+        <v>4</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>